<commit_message>
updated mappings from 2/8 workshop discussion
</commit_message>
<xml_diff>
--- a/Offsite Review/MDM Cloud Control Mapping.xlsx
+++ b/Offsite Review/MDM Cloud Control Mapping.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fisherj5\Desktop\New CCTL Projects\NIAP_CCPPD2\Cloud\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fisherj5\Desktop\Github\General\Offsite Review\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E608FCA-CEC8-46A8-B68E-3E75512CEB0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F443E3-A54B-416B-9A56-951E503E6CD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2778758D-9481-404F-8CA2-F24ED5DECC17}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{2778758D-9481-404F-8CA2-F24ED5DECC17}"/>
   </bookViews>
   <sheets>
     <sheet name="SFRs" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="262">
   <si>
     <t>SFR</t>
   </si>
@@ -675,9 +675,6 @@
     <t>Potentially applicable - testing for various platform functions may satisfy PP test activities in the case where an SFR is enforced through invocation of the platform function.</t>
   </si>
   <si>
-    <t>Potentially applicable - SSP documentaiton will include instructions for secure configuration of the platform. Adherence to this guidance may be needed to ensure that the TOE is deployed in an environment that is consistent with the PP's assumptions.</t>
-  </si>
-  <si>
     <t>Not applicable - validation of the underlying platform does not relate to the configuration management of the TOE.</t>
   </si>
   <si>
@@ -690,13 +687,7 @@
     <t>Applicable - FedRAMP penetration test guidance requires fairly extensive measures to demonstrate the platform's resistance to attack. At minimum, a validation of the platform provides assurance that the PP's assumptions about the security of the underlying platform are met (if assessed at FedRAMP Moderate or High). A separate vulnerability analysis of the MDM itself is still needed.</t>
   </si>
   <si>
-    <t xml:space="preserve">Availability of the cloud service (server up and running, boundary protection configured in such a way that connectivity isn't inhibited) </t>
-  </si>
-  <si>
     <t>Applicable Controls (C5)</t>
-  </si>
-  <si>
-    <t>SC-5 (protection against denial of service)</t>
   </si>
   <si>
     <t>FedRAMP Level</t>
@@ -832,16 +823,6 @@
 (source: https://www.fedramp.gov/assets/resources/documents/CSP_Penetration_Test_Guidance.pdf)</t>
   </si>
   <si>
-    <t xml:space="preserve">Review documentation/policies relating to service availability and historical data about service downtime
-Interview responsible personnel to determine how availability is mantained
-Test any mechanisms that protect against or limits the effects of DoS attacks
-</t>
-  </si>
-  <si>
-    <t>BC-04 (information on the availability of the data centre)
-COS-01 (protection against denial of service)</t>
-  </si>
-  <si>
     <t>OPS-10 (logging and monitoring - concept)</t>
   </si>
   <si>
@@ -883,6 +864,12 @@
   </si>
   <si>
     <t>To be added after applicable FedRAMP controls are determined</t>
+  </si>
+  <si>
+    <t>Potentially applicable - SSP documentation will include instructions for secure configuration of the platform. Adherence to this guidance may be needed to ensure that the TOE is deployed in an environment that is consistent with the PP's assumptions.</t>
+  </si>
+  <si>
+    <t>None - according to the PP this is mapped to the OE.WIRELESS_NETWORK objective, so this is only applicable to mobile devices being able to access the wireless.</t>
   </si>
 </sst>
 </file>
@@ -1027,7 +1014,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1057,7 +1044,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1089,9 +1076,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1409,8 +1393,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54A4433C-9A99-4C7D-BC27-CB25F780297F}">
   <dimension ref="A1:G105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1439,7 +1424,7 @@
         <v>6</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>8</v>
@@ -1461,8 +1446,8 @@
       <c r="D2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="22" t="s">
-        <v>264</v>
+      <c r="E2" s="11" t="s">
+        <v>259</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>10</v>
@@ -1484,7 +1469,7 @@
       <c r="D3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="22"/>
+      <c r="E3" s="11"/>
       <c r="F3" s="12" t="s">
         <v>18</v>
       </c>
@@ -1501,7 +1486,7 @@
       <c r="D4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="22"/>
+      <c r="E4" s="11"/>
       <c r="F4" s="12"/>
       <c r="G4" s="15"/>
     </row>
@@ -1514,7 +1499,7 @@
       <c r="D5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="22"/>
+      <c r="E5" s="11"/>
       <c r="F5" s="12"/>
       <c r="G5" s="15"/>
     </row>
@@ -1527,7 +1512,7 @@
       <c r="D6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="22"/>
+      <c r="E6" s="11"/>
       <c r="F6" s="12"/>
       <c r="G6" s="14"/>
     </row>
@@ -1544,7 +1529,7 @@
       <c r="D7" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E7" s="22"/>
+      <c r="E7" s="11"/>
       <c r="F7" s="6" t="s">
         <v>10</v>
       </c>
@@ -1565,7 +1550,7 @@
       <c r="D8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="22"/>
+      <c r="E8" s="11"/>
       <c r="F8" s="6" t="s">
         <v>18</v>
       </c>
@@ -1582,7 +1567,7 @@
       <c r="D9" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="22"/>
+      <c r="E9" s="11"/>
       <c r="F9" s="6" t="s">
         <v>18</v>
       </c>
@@ -1601,7 +1586,7 @@
       <c r="D10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="22"/>
+      <c r="E10" s="11"/>
       <c r="F10" s="13" t="s">
         <v>30</v>
       </c>
@@ -1618,7 +1603,7 @@
       <c r="D11" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="22"/>
+      <c r="E11" s="11"/>
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
     </row>
@@ -1635,7 +1620,7 @@
       <c r="D12" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="22"/>
+      <c r="E12" s="11"/>
       <c r="F12" s="13" t="s">
         <v>30</v>
       </c>
@@ -1652,7 +1637,7 @@
       <c r="D13" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="22"/>
+      <c r="E13" s="11"/>
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
     </row>
@@ -1669,7 +1654,7 @@
       <c r="D14" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="22"/>
+      <c r="E14" s="11"/>
       <c r="F14" s="6" t="s">
         <v>18</v>
       </c>
@@ -1690,7 +1675,7 @@
       <c r="D15" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="22"/>
+      <c r="E15" s="11"/>
       <c r="F15" s="6" t="s">
         <v>30</v>
       </c>
@@ -1711,7 +1696,7 @@
       <c r="D16" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="22"/>
+      <c r="E16" s="11"/>
       <c r="F16" s="6" t="s">
         <v>30</v>
       </c>
@@ -1732,7 +1717,7 @@
       <c r="D17" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="22"/>
+      <c r="E17" s="11"/>
       <c r="F17" s="6" t="s">
         <v>30</v>
       </c>
@@ -1753,7 +1738,7 @@
       <c r="D18" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E18" s="22"/>
+      <c r="E18" s="11"/>
       <c r="F18" s="6" t="s">
         <v>30</v>
       </c>
@@ -1774,7 +1759,7 @@
       <c r="D19" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="22"/>
+      <c r="E19" s="11"/>
       <c r="F19" s="6" t="s">
         <v>30</v>
       </c>
@@ -1795,12 +1780,12 @@
       <c r="D20" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E20" s="22"/>
+      <c r="E20" s="11"/>
       <c r="F20" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1812,7 +1797,7 @@
       <c r="D21" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E21" s="22"/>
+      <c r="E21" s="11"/>
       <c r="F21" s="14"/>
       <c r="G21" s="12"/>
     </row>
@@ -1829,7 +1814,7 @@
       <c r="D22" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E22" s="22"/>
+      <c r="E22" s="11"/>
       <c r="F22" s="13" t="s">
         <v>10</v>
       </c>
@@ -1846,7 +1831,7 @@
       <c r="D23" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E23" s="22"/>
+      <c r="E23" s="11"/>
       <c r="F23" s="15"/>
       <c r="G23" s="15"/>
     </row>
@@ -1859,7 +1844,7 @@
       <c r="D24" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E24" s="22"/>
+      <c r="E24" s="11"/>
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
     </row>
@@ -1876,7 +1861,7 @@
       <c r="D25" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E25" s="22"/>
+      <c r="E25" s="11"/>
       <c r="F25" s="13" t="s">
         <v>18</v>
       </c>
@@ -1893,7 +1878,7 @@
       <c r="D26" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E26" s="22"/>
+      <c r="E26" s="11"/>
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
     </row>
@@ -1910,7 +1895,7 @@
       <c r="D27" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E27" s="22"/>
+      <c r="E27" s="11"/>
       <c r="F27" s="13" t="s">
         <v>30</v>
       </c>
@@ -1927,7 +1912,7 @@
       <c r="D28" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E28" s="22"/>
+      <c r="E28" s="11"/>
       <c r="F28" s="15"/>
       <c r="G28" s="15"/>
     </row>
@@ -1940,7 +1925,7 @@
       <c r="D29" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E29" s="22"/>
+      <c r="E29" s="11"/>
       <c r="F29" s="14"/>
       <c r="G29" s="14"/>
     </row>
@@ -1957,7 +1942,7 @@
       <c r="D30" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E30" s="22"/>
+      <c r="E30" s="11"/>
       <c r="F30" s="6" t="s">
         <v>18</v>
       </c>
@@ -1978,7 +1963,7 @@
       <c r="D31" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E31" s="22"/>
+      <c r="E31" s="11"/>
       <c r="F31" s="13" t="s">
         <v>18</v>
       </c>
@@ -1995,7 +1980,7 @@
       <c r="D32" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E32" s="22"/>
+      <c r="E32" s="11"/>
       <c r="F32" s="14"/>
       <c r="G32" s="14"/>
     </row>
@@ -2012,7 +1997,7 @@
       <c r="D33" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E33" s="22"/>
+      <c r="E33" s="11"/>
       <c r="F33" s="13" t="s">
         <v>10</v>
       </c>
@@ -2029,7 +2014,7 @@
       <c r="D34" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E34" s="22"/>
+      <c r="E34" s="11"/>
       <c r="F34" s="15"/>
       <c r="G34" s="15"/>
     </row>
@@ -2042,7 +2027,7 @@
       <c r="D35" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E35" s="22"/>
+      <c r="E35" s="11"/>
       <c r="F35" s="15"/>
       <c r="G35" s="15"/>
     </row>
@@ -2055,7 +2040,7 @@
       <c r="D36" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E36" s="22"/>
+      <c r="E36" s="11"/>
       <c r="F36" s="15"/>
       <c r="G36" s="15"/>
     </row>
@@ -2068,7 +2053,7 @@
       <c r="D37" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E37" s="22"/>
+      <c r="E37" s="11"/>
       <c r="F37" s="14"/>
       <c r="G37" s="14"/>
     </row>
@@ -2085,7 +2070,7 @@
       <c r="D38" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E38" s="22"/>
+      <c r="E38" s="11"/>
       <c r="F38" s="13" t="s">
         <v>10</v>
       </c>
@@ -2102,7 +2087,7 @@
       <c r="D39" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E39" s="22"/>
+      <c r="E39" s="11"/>
       <c r="F39" s="14"/>
       <c r="G39" s="14"/>
     </row>
@@ -2119,7 +2104,7 @@
       <c r="D40" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E40" s="22"/>
+      <c r="E40" s="11"/>
       <c r="F40" s="6" t="s">
         <v>10</v>
       </c>
@@ -2140,7 +2125,7 @@
       <c r="D41" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E41" s="22"/>
+      <c r="E41" s="11"/>
       <c r="F41" s="6" t="s">
         <v>10</v>
       </c>
@@ -2161,7 +2146,7 @@
       <c r="D42" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E42" s="22"/>
+      <c r="E42" s="11"/>
       <c r="F42" s="13" t="s">
         <v>10</v>
       </c>
@@ -2178,7 +2163,7 @@
       <c r="D43" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E43" s="22"/>
+      <c r="E43" s="11"/>
       <c r="F43" s="14"/>
       <c r="G43" s="14"/>
     </row>
@@ -2195,7 +2180,7 @@
       <c r="D44" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E44" s="22"/>
+      <c r="E44" s="11"/>
       <c r="F44" s="6" t="s">
         <v>10</v>
       </c>
@@ -2216,7 +2201,7 @@
       <c r="D45" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E45" s="22"/>
+      <c r="E45" s="11"/>
       <c r="F45" s="6" t="s">
         <v>10</v>
       </c>
@@ -2237,7 +2222,7 @@
       <c r="D46" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E46" s="22"/>
+      <c r="E46" s="11"/>
       <c r="F46" s="13" t="s">
         <v>18</v>
       </c>
@@ -2254,7 +2239,7 @@
       <c r="D47" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E47" s="22"/>
+      <c r="E47" s="11"/>
       <c r="F47" s="15"/>
       <c r="G47" s="15"/>
     </row>
@@ -2267,7 +2252,7 @@
       <c r="D48" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E48" s="22"/>
+      <c r="E48" s="11"/>
       <c r="F48" s="15"/>
       <c r="G48" s="15"/>
     </row>
@@ -2280,7 +2265,7 @@
       <c r="D49" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E49" s="22"/>
+      <c r="E49" s="11"/>
       <c r="F49" s="14"/>
       <c r="G49" s="14"/>
     </row>
@@ -2297,7 +2282,7 @@
       <c r="D50" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E50" s="22"/>
+      <c r="E50" s="11"/>
       <c r="F50" s="13" t="s">
         <v>18</v>
       </c>
@@ -2314,7 +2299,7 @@
       <c r="D51" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E51" s="22"/>
+      <c r="E51" s="11"/>
       <c r="F51" s="14"/>
       <c r="G51" s="14"/>
     </row>
@@ -2331,7 +2316,7 @@
       <c r="D52" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E52" s="22"/>
+      <c r="E52" s="11"/>
       <c r="F52" s="13" t="s">
         <v>10</v>
       </c>
@@ -2348,7 +2333,7 @@
       <c r="D53" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E53" s="22"/>
+      <c r="E53" s="11"/>
       <c r="F53" s="15"/>
       <c r="G53" s="15"/>
     </row>
@@ -2361,7 +2346,7 @@
       <c r="D54" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E54" s="22"/>
+      <c r="E54" s="11"/>
       <c r="F54" s="14"/>
       <c r="G54" s="14"/>
     </row>
@@ -2378,7 +2363,7 @@
       <c r="D55" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E55" s="22"/>
+      <c r="E55" s="11"/>
       <c r="F55" s="13" t="s">
         <v>18</v>
       </c>
@@ -2395,7 +2380,7 @@
       <c r="D56" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E56" s="22"/>
+      <c r="E56" s="11"/>
       <c r="F56" s="15"/>
       <c r="G56" s="15"/>
     </row>
@@ -2408,7 +2393,7 @@
       <c r="D57" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E57" s="22"/>
+      <c r="E57" s="11"/>
       <c r="F57" s="14"/>
       <c r="G57" s="14"/>
     </row>
@@ -2425,7 +2410,7 @@
       <c r="D58" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E58" s="22"/>
+      <c r="E58" s="11"/>
       <c r="F58" s="13" t="s">
         <v>18</v>
       </c>
@@ -2442,7 +2427,7 @@
       <c r="D59" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E59" s="22"/>
+      <c r="E59" s="11"/>
       <c r="F59" s="14"/>
       <c r="G59" s="14"/>
     </row>
@@ -2459,7 +2444,7 @@
       <c r="D60" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E60" s="22"/>
+      <c r="E60" s="11"/>
       <c r="F60" s="13" t="s">
         <v>18</v>
       </c>
@@ -2476,7 +2461,7 @@
       <c r="D61" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E61" s="22"/>
+      <c r="E61" s="11"/>
       <c r="F61" s="14"/>
       <c r="G61" s="14"/>
     </row>
@@ -2493,7 +2478,7 @@
       <c r="D62" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="E62" s="22"/>
+      <c r="E62" s="11"/>
       <c r="F62" s="13" t="s">
         <v>18</v>
       </c>
@@ -2510,7 +2495,7 @@
       <c r="D63" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E63" s="22"/>
+      <c r="E63" s="11"/>
       <c r="F63" s="14"/>
       <c r="G63" s="14"/>
     </row>
@@ -2527,7 +2512,7 @@
       <c r="D64" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E64" s="22"/>
+      <c r="E64" s="11"/>
       <c r="F64" s="6" t="s">
         <v>18</v>
       </c>
@@ -2548,7 +2533,7 @@
       <c r="D65" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E65" s="22"/>
+      <c r="E65" s="11"/>
       <c r="F65" s="6" t="s">
         <v>18</v>
       </c>
@@ -2569,7 +2554,7 @@
       <c r="D66" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E66" s="22"/>
+      <c r="E66" s="11"/>
       <c r="F66" s="13" t="s">
         <v>18</v>
       </c>
@@ -2586,7 +2571,7 @@
       <c r="D67" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E67" s="22"/>
+      <c r="E67" s="11"/>
       <c r="F67" s="15"/>
       <c r="G67" s="15"/>
     </row>
@@ -2599,7 +2584,7 @@
       <c r="D68" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E68" s="22"/>
+      <c r="E68" s="11"/>
       <c r="F68" s="15"/>
       <c r="G68" s="15"/>
     </row>
@@ -2612,7 +2597,7 @@
       <c r="D69" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E69" s="22"/>
+      <c r="E69" s="11"/>
       <c r="F69" s="14"/>
       <c r="G69" s="14"/>
     </row>
@@ -2629,7 +2614,7 @@
       <c r="D70" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E70" s="22"/>
+      <c r="E70" s="11"/>
       <c r="F70" s="6" t="s">
         <v>18</v>
       </c>
@@ -2650,7 +2635,7 @@
       <c r="D71" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E71" s="22"/>
+      <c r="E71" s="11"/>
       <c r="F71" s="13" t="s">
         <v>10</v>
       </c>
@@ -2667,7 +2652,7 @@
       <c r="D72" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E72" s="22"/>
+      <c r="E72" s="11"/>
       <c r="F72" s="15"/>
       <c r="G72" s="15"/>
     </row>
@@ -2680,7 +2665,7 @@
       <c r="D73" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E73" s="22"/>
+      <c r="E73" s="11"/>
       <c r="F73" s="14"/>
       <c r="G73" s="14"/>
     </row>
@@ -2697,7 +2682,7 @@
       <c r="D74" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E74" s="22"/>
+      <c r="E74" s="11"/>
       <c r="F74" s="6" t="s">
         <v>18</v>
       </c>
@@ -2718,7 +2703,7 @@
       <c r="D75" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E75" s="22"/>
+      <c r="E75" s="11"/>
       <c r="F75" s="13" t="s">
         <v>30</v>
       </c>
@@ -2735,7 +2720,7 @@
       <c r="D76" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E76" s="22"/>
+      <c r="E76" s="11"/>
       <c r="F76" s="15"/>
       <c r="G76" s="15"/>
     </row>
@@ -2748,7 +2733,7 @@
       <c r="D77" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E77" s="22"/>
+      <c r="E77" s="11"/>
       <c r="F77" s="15"/>
       <c r="G77" s="15"/>
     </row>
@@ -2761,7 +2746,7 @@
       <c r="D78" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E78" s="22"/>
+      <c r="E78" s="11"/>
       <c r="F78" s="14"/>
       <c r="G78" s="14"/>
     </row>
@@ -2778,7 +2763,7 @@
       <c r="D79" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E79" s="22"/>
+      <c r="E79" s="11"/>
       <c r="F79" s="13" t="s">
         <v>30</v>
       </c>
@@ -2795,7 +2780,7 @@
       <c r="D80" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E80" s="22"/>
+      <c r="E80" s="11"/>
       <c r="F80" s="15"/>
       <c r="G80" s="15"/>
     </row>
@@ -2808,7 +2793,7 @@
       <c r="D81" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E81" s="22"/>
+      <c r="E81" s="11"/>
       <c r="F81" s="14"/>
       <c r="G81" s="14"/>
     </row>
@@ -2825,7 +2810,7 @@
       <c r="D82" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E82" s="22"/>
+      <c r="E82" s="11"/>
       <c r="F82" s="13" t="s">
         <v>10</v>
       </c>
@@ -2842,7 +2827,7 @@
       <c r="D83" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E83" s="22"/>
+      <c r="E83" s="11"/>
       <c r="F83" s="14"/>
       <c r="G83" s="14"/>
     </row>
@@ -2859,7 +2844,7 @@
       <c r="D84" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E84" s="22"/>
+      <c r="E84" s="11"/>
       <c r="F84" s="6" t="s">
         <v>10</v>
       </c>
@@ -2880,7 +2865,7 @@
       <c r="D85" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E85" s="22"/>
+      <c r="E85" s="11"/>
       <c r="F85" s="6" t="s">
         <v>10</v>
       </c>
@@ -2901,7 +2886,7 @@
       <c r="D86" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E86" s="22"/>
+      <c r="E86" s="11"/>
       <c r="F86" s="13" t="s">
         <v>18</v>
       </c>
@@ -2918,7 +2903,7 @@
       <c r="D87" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E87" s="22"/>
+      <c r="E87" s="11"/>
       <c r="F87" s="14"/>
       <c r="G87" s="14"/>
     </row>
@@ -2935,7 +2920,7 @@
       <c r="D88" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E88" s="22"/>
+      <c r="E88" s="11"/>
       <c r="F88" s="13" t="s">
         <v>18</v>
       </c>
@@ -2952,7 +2937,7 @@
       <c r="D89" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E89" s="22"/>
+      <c r="E89" s="11"/>
       <c r="F89" s="15"/>
       <c r="G89" s="15"/>
     </row>
@@ -2965,7 +2950,7 @@
       <c r="D90" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E90" s="22"/>
+      <c r="E90" s="11"/>
       <c r="F90" s="14"/>
       <c r="G90" s="14"/>
     </row>
@@ -2982,7 +2967,7 @@
       <c r="D91" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E91" s="22"/>
+      <c r="E91" s="11"/>
       <c r="F91" s="13" t="s">
         <v>18</v>
       </c>
@@ -2999,7 +2984,7 @@
       <c r="D92" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E92" s="22"/>
+      <c r="E92" s="11"/>
       <c r="F92" s="15"/>
       <c r="G92" s="15"/>
     </row>
@@ -3012,7 +2997,7 @@
       <c r="D93" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E93" s="22"/>
+      <c r="E93" s="11"/>
       <c r="F93" s="14"/>
       <c r="G93" s="14"/>
     </row>
@@ -3029,7 +3014,7 @@
       <c r="D94" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E94" s="22"/>
+      <c r="E94" s="11"/>
       <c r="F94" s="13" t="s">
         <v>10</v>
       </c>
@@ -3046,7 +3031,7 @@
       <c r="D95" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E95" s="22"/>
+      <c r="E95" s="11"/>
       <c r="F95" s="15"/>
       <c r="G95" s="15"/>
     </row>
@@ -3059,7 +3044,7 @@
       <c r="D96" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E96" s="22"/>
+      <c r="E96" s="11"/>
       <c r="F96" s="15"/>
       <c r="G96" s="15"/>
     </row>
@@ -3072,7 +3057,7 @@
       <c r="D97" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E97" s="22"/>
+      <c r="E97" s="11"/>
       <c r="F97" s="14"/>
       <c r="G97" s="14"/>
     </row>
@@ -3089,7 +3074,7 @@
       <c r="D98" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E98" s="22"/>
+      <c r="E98" s="11"/>
       <c r="F98" s="6" t="s">
         <v>18</v>
       </c>
@@ -3110,7 +3095,7 @@
       <c r="D99" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E99" s="22"/>
+      <c r="E99" s="11"/>
       <c r="F99" s="6" t="s">
         <v>10</v>
       </c>
@@ -3131,7 +3116,7 @@
       <c r="D100" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E100" s="22"/>
+      <c r="E100" s="11"/>
       <c r="F100" s="6" t="s">
         <v>10</v>
       </c>
@@ -3152,7 +3137,7 @@
       <c r="D101" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E101" s="22"/>
+      <c r="E101" s="11"/>
       <c r="F101" s="6" t="s">
         <v>30</v>
       </c>
@@ -3173,7 +3158,7 @@
       <c r="D102" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E102" s="22"/>
+      <c r="E102" s="11"/>
       <c r="F102" s="6" t="s">
         <v>10</v>
       </c>
@@ -3194,7 +3179,7 @@
       <c r="D103" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E103" s="22"/>
+      <c r="E103" s="11"/>
       <c r="F103" s="6" t="s">
         <v>10</v>
       </c>
@@ -3215,7 +3200,7 @@
       <c r="D104" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E104" s="22"/>
+      <c r="E104" s="11"/>
       <c r="F104" s="13" t="s">
         <v>18</v>
       </c>
@@ -3232,7 +3217,7 @@
       <c r="D105" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E105" s="22"/>
+      <c r="E105" s="11"/>
       <c r="F105" s="14"/>
       <c r="G105" s="14"/>
     </row>
@@ -3363,8 +3348,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94B24DA9-4BA3-4ECC-9FAB-E70DCA771AAE}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="A3" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3386,7 +3371,7 @@
         <v>198</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -3394,7 +3379,7 @@
         <v>199</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -3402,7 +3387,7 @@
         <v>200</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>207</v>
+        <v>260</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3410,7 +3395,7 @@
         <v>201</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3418,7 +3403,7 @@
         <v>202</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3434,7 +3419,7 @@
         <v>204</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -3447,8 +3432,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FBB7BE9-4435-40AA-8EE2-4971B8BFFA64}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3478,13 +3464,13 @@
         <v>60</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>61</v>
@@ -3516,7 +3502,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>51</v>
       </c>
@@ -3524,22 +3510,22 @@
         <v>58</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>212</v>
+        <v>261</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>214</v>
+        <v>63</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>252</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>251</v>
+        <v>63</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3553,7 +3539,7 @@
         <v>17</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="E4" s="16"/>
       <c r="F4" s="17"/>
@@ -3565,19 +3551,19 @@
       <c r="B5" s="15"/>
       <c r="C5" s="20"/>
       <c r="D5" s="6" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="120" x14ac:dyDescent="0.25">
@@ -3585,19 +3571,19 @@
       <c r="B6" s="15"/>
       <c r="C6" s="20"/>
       <c r="D6" s="6" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>19</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="120" x14ac:dyDescent="0.25">
@@ -3605,7 +3591,7 @@
       <c r="B7" s="15"/>
       <c r="C7" s="20"/>
       <c r="D7" s="6" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>38</v>
@@ -3614,10 +3600,10 @@
         <v>19</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="90" x14ac:dyDescent="0.25">
@@ -3625,19 +3611,19 @@
       <c r="B8" s="15"/>
       <c r="C8" s="20"/>
       <c r="D8" s="6" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>19</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="120" x14ac:dyDescent="0.25">
@@ -3645,19 +3631,19 @@
       <c r="B9" s="15"/>
       <c r="C9" s="20"/>
       <c r="D9" s="6" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="135" x14ac:dyDescent="0.25">
@@ -3665,19 +3651,19 @@
       <c r="B10" s="14"/>
       <c r="C10" s="21"/>
       <c r="D10" s="6" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="165" x14ac:dyDescent="0.25">
@@ -3691,7 +3677,7 @@
         <v>17</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="E11" s="16"/>
       <c r="F11" s="17"/>
@@ -3703,7 +3689,7 @@
       <c r="B12" s="15"/>
       <c r="C12" s="20"/>
       <c r="D12" s="6" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>38</v>
@@ -3712,10 +3698,10 @@
         <v>19</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="120" x14ac:dyDescent="0.25">
@@ -3723,19 +3709,19 @@
       <c r="B13" s="15"/>
       <c r="C13" s="20"/>
       <c r="D13" s="6" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="195" x14ac:dyDescent="0.25">
@@ -3743,19 +3729,19 @@
       <c r="B14" s="15"/>
       <c r="C14" s="20"/>
       <c r="D14" s="6" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>20</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="330" x14ac:dyDescent="0.25">
@@ -3763,19 +3749,19 @@
       <c r="B15" s="14"/>
       <c r="C15" s="21"/>
       <c r="D15" s="6" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>20</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="60" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updating MDM mapping doc (assumptions tab) based on discussions at CCitC workshop
</commit_message>
<xml_diff>
--- a/Offsite Review/MDM Cloud Control Mapping.xlsx
+++ b/Offsite Review/MDM Cloud Control Mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fisherj5\Desktop\Github\General\Offsite Review\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F443E3-A54B-416B-9A56-951E503E6CD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6838862-5B88-409C-873D-D4EDEA0E4B02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{2778758D-9481-404F-8CA2-F24ED5DECC17}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{2778758D-9481-404F-8CA2-F24ED5DECC17}"/>
   </bookViews>
   <sheets>
     <sheet name="SFRs" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="279">
   <si>
     <t>SFR</t>
   </si>
@@ -734,12 +734,6 @@
     <t>prevention of unauthorized physical access</t>
   </si>
   <si>
-    <t>enforcement of separation mechanisms if multi-tenant platform is used</t>
-  </si>
-  <si>
-    <t>penetration testing to show prevention of unauthorized access and protection against privilege escalation</t>
-  </si>
-  <si>
     <t>CA-8</t>
   </si>
   <si>
@@ -770,9 +764,6 @@
   <si>
     <t>AU-9 Low
 AU-9(2) Moderate</t>
-  </si>
-  <si>
-    <t>SC-7(12) Moderate</t>
   </si>
   <si>
     <t>Review documentation that describes how accurate system time is maintained, including any guidance for NTP synchronization
@@ -850,9 +841,6 @@
     <t>OPS-23 (managing vulnerabilities, malfunctions, and errors - system hardening)</t>
   </si>
   <si>
-    <t>PSS-09 (authorisation mechanisms)</t>
-  </si>
-  <si>
     <t>COS-02 (security requirements for connections in the cloud service provider's network)
 COS-06 (segregation of data traffic in jointly used network environments)
 DEV-03 (policies for changes to information systems)
@@ -870,6 +858,74 @@
   </si>
   <si>
     <t>None - according to the PP this is mapped to the OE.WIRELESS_NETWORK objective, so this is only applicable to mobile devices being able to access the wireless.</t>
+  </si>
+  <si>
+    <t>enforcement of isolation/segmentation mechanism between MDM and other customers using the same platforms</t>
+  </si>
+  <si>
+    <t>penetration testing for the platform to show prevention of unauthorized access and protection against privilege escalation</t>
+  </si>
+  <si>
+    <t>protection of data in transit</t>
+  </si>
+  <si>
+    <t>protection of stored data at rest (specifically private keys)</t>
+  </si>
+  <si>
+    <t>SC-28, SC-28(3)</t>
+  </si>
+  <si>
+    <t>SC-28 Moderate
+SC-28(3) N/A</t>
+  </si>
+  <si>
+    <t>Identify through documentation what trusted communications protocols are used to protected data in transit. 
+Ensure through testing that the interface for these protocols can be invoked and that the use of insecure or unauthorized protocols can be restricted.</t>
+  </si>
+  <si>
+    <t>Identify the protection mechanism used to ensure the confidentiality and integrity of data at rest.
+Ensure through testing that this mechanism can be used to store the desired data.</t>
+  </si>
+  <si>
+    <t>CRY-02 (encryption of data for transmission (transport encryption))</t>
+  </si>
+  <si>
+    <t>CRY-04 (secure key management)</t>
+  </si>
+  <si>
+    <t>Uncategorized</t>
+  </si>
+  <si>
+    <t>COS-01 (technical safeguards)
+PSS-09 (authorisation mechanisms)</t>
+  </si>
+  <si>
+    <t>SC-28, SC-28(1)</t>
+  </si>
+  <si>
+    <t>SC-28 Moderate
+SC-28(1) Moderate</t>
+  </si>
+  <si>
+    <t>Functionality that does not relate to any specific assumptions or environmental objectives in the PP but may be considered as controls a platform needs to implement to show a baseline level of trustworthiness can be achieved by the platform.</t>
+  </si>
+  <si>
+    <t>use of digital signature services to validate software integrity prior to installation/deployment</t>
+  </si>
+  <si>
+    <t>N/A - PSS-11 (images for virtual machines and containers) talks about integrity checks for VMs and container images at startup/runtime but nothing related to the integrity of a SaaS deployed on such a platform</t>
+  </si>
+  <si>
+    <t>Unknown - no apparent explicit control that relates to the cloud service provider's role in ensuring that data generated or consumed by a SaaS is protected while at rest</t>
+  </si>
+  <si>
+    <t>Ensure that an unsigned or incorrectly signed distribution of a product cannot successfully be deployed on the cloud platform</t>
+  </si>
+  <si>
+    <t>use of platform services to provide protection of data at rest</t>
+  </si>
+  <si>
+    <t>Identify the mechanisms used for storage of data at rest and how confidentiality of that data is maintaned</t>
   </si>
 </sst>
 </file>
@@ -1014,7 +1070,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1075,6 +1131,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1447,7 +1506,7 @@
         <v>20</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>10</v>
@@ -1785,7 +1844,7 @@
         <v>18</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3387,7 +3446,7 @@
         <v>200</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -3430,11 +3489,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FBB7BE9-4435-40AA-8EE2-4971B8BFFA64}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3513,7 +3572,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>63</v>
@@ -3557,13 +3616,13 @@
         <v>215</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="120" x14ac:dyDescent="0.25">
@@ -3580,10 +3639,10 @@
         <v>19</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="120" x14ac:dyDescent="0.25">
@@ -3600,10 +3659,10 @@
         <v>19</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="90" x14ac:dyDescent="0.25">
@@ -3614,16 +3673,16 @@
         <v>221</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>19</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>256</v>
+        <v>269</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="120" x14ac:dyDescent="0.25">
@@ -3634,22 +3693,22 @@
         <v>222</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="135" x14ac:dyDescent="0.25">
-      <c r="A10" s="21"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="21"/>
+      <c r="A10" s="20"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="20"/>
       <c r="D10" s="6" t="s">
         <v>223</v>
       </c>
@@ -3657,111 +3716,111 @@
         <v>217</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>237</v>
+        <v>20</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="165" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A11" s="20"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12" s="21"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+      <c r="A13" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B13" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C13" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D13" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="E11" s="16"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="18"/>
-    </row>
-    <row r="12" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="H12" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="120" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="6" t="s">
-        <v>225</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>231</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>254</v>
-      </c>
-      <c r="H13" s="10" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="195" x14ac:dyDescent="0.25">
+      <c r="E13" s="16"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="18"/>
+    </row>
+    <row r="14" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A14" s="20"/>
       <c r="B14" s="15"/>
       <c r="C14" s="20"/>
       <c r="D14" s="6" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>230</v>
+        <v>38</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="330" x14ac:dyDescent="0.25">
-      <c r="A15" s="21"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="21"/>
+        <v>241</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A15" s="20"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="20"/>
       <c r="D15" s="6" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>20</v>
+        <v>231</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3790,16 +3849,110 @@
         <v>63</v>
       </c>
     </row>
+    <row r="17" spans="1:8" ht="330" x14ac:dyDescent="0.25">
+      <c r="A17" s="22" t="s">
+        <v>268</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A18" s="22"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="195" x14ac:dyDescent="0.25">
+      <c r="A19" s="22"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A20" s="22"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>278</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="B17:B20"/>
     <mergeCell ref="E4:H4"/>
-    <mergeCell ref="E11:H11"/>
-    <mergeCell ref="A4:A10"/>
-    <mergeCell ref="B4:B10"/>
-    <mergeCell ref="C4:C10"/>
-    <mergeCell ref="A11:A15"/>
-    <mergeCell ref="B11:B15"/>
-    <mergeCell ref="C11:C15"/>
+    <mergeCell ref="E13:H13"/>
+    <mergeCell ref="A4:A12"/>
+    <mergeCell ref="B4:B12"/>
+    <mergeCell ref="C4:C12"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="C13:C15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>